<commit_message>
📝 docs(other): Update the interface definition file for Chapter 1
</commit_message>
<xml_diff>
--- a/static/asset/rdk_s100/drobotics_rdk_s100_camera_expansion_board_pinlist_v1p0-eng.xlsx
+++ b/static/asset/rdk_s100/drobotics_rdk_s100_camera_expansion_board_pinlist_v1p0-eng.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoye.zhang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\需求备份\杨高明-1120-httpshorizonrobotics.feishu.cnwikiV7K4wCRHNiaSufk0Otcceqaen2c\替换掉的原表格备份\新表格\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="79">
   <si>
     <t>Pin No</t>
   </si>
@@ -210,6 +210,10 @@
   </si>
   <si>
     <t>MIPI_RX1_DN0_B0</t>
+  </si>
+  <si>
+    <t>MIPI Camera 1 Interface Definition (J2200)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Function Description</t>
@@ -279,13 +283,47 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Function 0: PU,10K
-Function 1: /</t>
+    <t>Function 0：PU,10K
+Function 1：/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <t>MIPI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Camera 2 Interface Definition(J2201)</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function Description</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logic Level</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Direction</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> MIPI Camera 3.3V Power Supply</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>MIPI Camera I2C SDA</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -307,24 +345,39 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>I2C SCL</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIPI Camera 1 Interface Definition (J2200)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIPI Camera LPWM or MCLK Signal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> MIPI Camera Enable Control</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">MIPI Camera </t>
+      <t>Function 0：PU,10K</t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
@@ -332,27 +385,26 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2</t>
+      <t xml:space="preserve">Function </t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Interface Definition(J2201)</t>
+      <t>1：/</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,7 +434,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
@@ -391,6 +449,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
@@ -524,47 +583,47 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,559 +1107,558 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.26953125" style="14"/>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="28.08984375" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" customWidth="1"/>
+    <col min="7" max="7" width="36.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:7" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="C3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>7</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="G23" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>13</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>14</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>16</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>17</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>18</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>19</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>20</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>21</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>22</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1618,31 +1676,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="28.08984375" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
     <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+    <row r="1" spans="1:7" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1651,525 +1709,525 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>61</v>
+      <c r="E2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="C3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>67</v>
+      <c r="G7" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="8" t="s">
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="8" t="s">
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="E23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2177,8 +2235,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>